<commit_message>
Added and updated tests for all changed code and fixed the file name used in PeakAnnotationsLoader.missing_annot_file_details.
Details:

- Added tests:
  - test_report_discrepant_headers_blank_with_missing_annot
  - test_report_discrepant_headers_blank_with_present_annot
  - test_initialize_msrun_data_annot_file_absent
- Updated test: test_study_loader_create_grouped_exceptions
- PeakAnnotationsLoader
  - Changed the filename added to instance member missing_annot_file_details to be the peak annotation filename as opposed to the study doc supplied to the contained MSRunsLoader.  A test revealed that it was the wrong file.

Files checked in: DataRepo/data/tests/submission_v3/multitracer_v3/study_missing_data.xlsx DataRepo/loaders/peak_annotations_loader.py DataRepo/tests/loaders/test_peak_annotations_loader.py DataRepo/tests/loaders/test_study_loader.py
</commit_message>
<xml_diff>
--- a/DataRepo/data/tests/submission_v3/multitracer_v3/study_missing_data.xlsx
+++ b/DataRepo/data/tests/submission_v3/multitracer_v3/study_missing_data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10916"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10208"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rleach/PROJECT-LOCAL/TRACEBASE/tracebase/DataRepo/data/tests/submission_v3/multitracer_v3/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{866121C3-1A9A-5B4D-87D0-B94BCDEF5A6E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B92EDFD0-031E-A648-9B89-089CC177EE35}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7280" yWindow="4920" windowWidth="39940" windowHeight="21040" tabRatio="500" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2540" yWindow="2400" windowWidth="39940" windowHeight="21040" tabRatio="500" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Study" sheetId="5" r:id="rId1"/>
@@ -27,8 +27,19 @@
     <sheet name="Peak Annotation Details" sheetId="12" r:id="rId12"/>
     <sheet name="Defaults" sheetId="13" r:id="rId13"/>
   </sheets>
-  <calcPr calcId="0" iterateDelta="1E-4"/>
+  <calcPr calcId="191029"/>
   <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="CalcA1ExcelA1"/>
     </ext>
@@ -1343,9 +1354,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9072829C-D118-B24B-B49F-A037A59AEB40}">
   <dimension ref="A1:K2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>

</xml_diff>